<commit_message>
[ ADD SPACE AFTER BA_DEF_ STRING ] [ ADD VECTOR_LEERSTRING FOR EMPTY STRING ]
</commit_message>
<xml_diff>
--- a/dbc/CAN_VARIANT/Comfort.xlsx
+++ b/dbc/CAN_VARIANT/Comfort.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3002" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3000" uniqueCount="318">
   <si>
     <t>Result</t>
   </si>
@@ -7706,11 +7706,11 @@
       <c r="C16" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>46</v>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1000000</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>

</xml_diff>